<commit_message>
add new data for training
* update the data and stock list
* only 000672 cannot be download since the data on the website is wrong
</commit_message>
<xml_diff>
--- a/data/raw/stock list.xlsx
+++ b/data/raw/stock list.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-36360" yWindow="1120" windowWidth="16120" windowHeight="14800" tabRatio="500"/>
+    <workbookView xWindow="-35980" yWindow="1000" windowWidth="16120" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="240">
   <si>
     <t>所属板块</t>
     <rPh sb="0" eb="1">
@@ -253,18 +253,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>再升科技</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>玻璃陶瓷</t>
     <rPh sb="0" eb="1">
       <t>bo li tao ci</t>
     </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>603601</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -665,17 +657,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>300581</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>晨曦航空</t>
-    <rPh sb="0" eb="1">
-      <t>chen xi hang kong</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>002230</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -900,17 +881,6 @@
     <t>中航电测</t>
     <rPh sb="0" eb="1">
       <t>zhong hang dian ce</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>300498</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>温室股份</t>
-    <rPh sb="0" eb="1">
-      <t>wen shi gu fen</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1152,6 +1122,291 @@
     <t>江河集团</t>
     <rPh sb="0" eb="1">
       <t>jiang he ji tuan</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2011.09.30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600288</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大恒科技</t>
+    <rPh sb="0" eb="1">
+      <t>da heng ke ji</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002577</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷柏科技</t>
+    <rPh sb="0" eb="1">
+      <t>lei bo ke ji</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002413</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷科防务</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000977</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>浪潮信息</t>
+    <rPh sb="0" eb="1">
+      <t>lang chao xin xi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002161</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远望谷</t>
+    <rPh sb="0" eb="1">
+      <t>yuan wang gu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600054</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄山旅游</t>
+    <rPh sb="0" eb="1">
+      <t>huang shan lü you</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>旅游酒店</t>
+    <rPh sb="0" eb="1">
+      <t>lü you jiu dian</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600593</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大连圣亚</t>
+    <rPh sb="0" eb="1">
+      <t>da lian sheng ya</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000430</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张家界</t>
+    <rPh sb="0" eb="1">
+      <t>zhang jia jie</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300144</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宋城演艺</t>
+    <rPh sb="0" eb="1">
+      <t>song cheng yan yi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000626</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>远大控股</t>
+    <rPh sb="0" eb="1">
+      <t>yuan da kong gu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>国际贸易</t>
+    <rPh sb="0" eb="1">
+      <t>guo ji mao yi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600278</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>东方创业</t>
+    <rPh sb="0" eb="1">
+      <t>dong fang chuang ye</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000554</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>泰山石油</t>
+    <rPh sb="0" eb="1">
+      <t>tai shan shi you</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>石油行业</t>
+    <rPh sb="0" eb="1">
+      <t>shi you hang ye</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>601808</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中海油服</t>
+    <rPh sb="0" eb="1">
+      <t>zhong hai you fu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机械行业</t>
+  </si>
+  <si>
+    <t>机械行业</t>
+    <rPh sb="0" eb="1">
+      <t>ji xie hang ye</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中兵红箭</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机器人</t>
+    <rPh sb="0" eb="1">
+      <t>ji qi ren</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>大洋电机</t>
+    <rPh sb="0" eb="1">
+      <t>da yang dian ji</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三一重工</t>
+    <rPh sb="0" eb="1">
+      <t>san yi zhong gong</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000519</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>300024</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002249</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002300</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>太阳电缆</t>
+    <rPh sb="0" eb="1">
+      <t>tai yang dian lan</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>002364</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>中恒电气</t>
+    <rPh sb="0" eb="1">
+      <t>zhong heng dian qi</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>电器行业</t>
+    <rPh sb="0" eb="1">
+      <t>dian qi hang ye</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600662</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>强生控股</t>
+    <rPh sb="0" eb="1">
+      <t>qiang sheng kong gu</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600703</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三安光电</t>
+    <rPh sb="0" eb="1">
+      <t>san an guang dian</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>贵州茅台</t>
+    <rPh sb="0" eb="1">
+      <t>gui zhou mao tai</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>600519</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>000858</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>五粮液</t>
+    <rPh sb="0" eb="1">
+      <t>wu liang ye</t>
     </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1160,7 +1415,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1189,6 +1444,29 @@
       <color rgb="FFFF0000"/>
       <name val="Abadi MT Condensed Extra Bold"/>
     </font>
+    <font>
+      <sz val="11.75"/>
+      <color rgb="FFFF0000"/>
+      <name val="Abadi MT Condensed Extra Bold"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1213,10 +1491,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1229,9 +1509,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1248,11 +1525,34 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1527,10 +1827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D91"/>
+  <dimension ref="A1:D150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="D87" sqref="A87:D87"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1580,25 +1880,25 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A4" s="7">
+      <c r="A4" s="13">
         <v>600690</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A5" s="7">
+      <c r="A5" s="13">
         <v>600337</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="13" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="1"/>
@@ -1616,25 +1916,25 @@
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="1"/>
@@ -1696,13 +1996,13 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="13" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="1"/>
@@ -1717,743 +2017,725 @@
       <c r="C14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="8">
         <v>20110408</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A16" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D16" s="1">
-        <v>20150130</v>
-      </c>
+      <c r="A16" s="12"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="C18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A18" s="8" t="s">
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A19" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B20" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="7" t="s">
+      <c r="C20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A21" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="8" t="s">
+      <c r="C21" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A22" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>40</v>
+      <c r="C22" s="13" t="s">
+        <v>38</v>
       </c>
       <c r="D22" s="1"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>51</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>53</v>
       </c>
       <c r="D23" s="1"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A25" s="8" t="s">
+      <c r="C25" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A26" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B25" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A26" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>53</v>
+      <c r="C26" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="D26" s="1"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A27" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="1"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="D28" s="1"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A29" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="B29" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A29" s="8" t="s">
+      <c r="C29" s="13" t="s">
         <v>64</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="D29" s="1"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A30" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D30" s="1"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A31" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D31" s="1"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A32" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D32" s="1"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A33" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D33" s="1"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A34" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B34" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>78</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A35" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>81</v>
       </c>
       <c r="D35" s="1"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A36" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A37" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D37" s="1"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A38" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="C37" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A38" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>84</v>
+      <c r="C38" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="D38" s="1"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A39" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D39" s="1"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A40" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D40" s="1"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A41" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A42" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A43" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A44" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="D44" s="1"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A45" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="B45" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A45" s="8" t="s">
+      <c r="C45" s="13" t="s">
         <v>102</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="D45" s="1"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A46" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B46" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A47" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>107</v>
-      </c>
+      <c r="A47" s="12"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="13"/>
       <c r="D47" s="1"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A48" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D48" s="1"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A49" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D49" s="1"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A50" s="3" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D50" s="1"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A51" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D51" s="1"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A52" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C52" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="D52" s="1"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A54" s="5" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A55" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A56" s="5" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A57" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A58" s="5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A60" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A61" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="B60" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="C60" s="4" t="s">
+      <c r="C61" s="13" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B61" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C61" s="7" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A63" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A64" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A65" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="B65" s="7" t="s">
-        <v>150</v>
-      </c>
-      <c r="C65" s="7" t="s">
-        <v>151</v>
-      </c>
+      <c r="A65" s="14"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="13"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A66" s="5" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A67" s="2"/>
     </row>
     <row r="68" spans="1:4" ht="16" x14ac:dyDescent="0.15">
-      <c r="A68" s="11" t="s">
+      <c r="A68" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="B68" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C68" s="11"/>
+      <c r="D68" s="11">
+        <v>20100730</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A69" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="11">
+        <v>20091030</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A70" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C70" s="11"/>
+      <c r="D70" s="11"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A71" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="B71" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="C68" s="12"/>
-      <c r="D68" s="12">
-        <v>20100730</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="11" t="s">
+      <c r="C71" s="11"/>
+      <c r="D71" s="11"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B69" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C69" s="12"/>
-      <c r="D69" s="12">
-        <v>20091030</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A70" s="11" t="s">
+      <c r="C72" s="11"/>
+      <c r="D72" s="11">
+        <v>20070831</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A73" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="B70" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="C70" s="12"/>
-      <c r="D70" s="12"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="11" t="s">
+      <c r="C73" s="11"/>
+      <c r="D73" s="11"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A74" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B74" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C74" s="11"/>
+      <c r="D74" s="11">
+        <v>20110630</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A75" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C75" s="11"/>
+      <c r="D75" s="11">
+        <v>20080530</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A76" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="C76" s="11"/>
+      <c r="D76" s="11">
+        <v>20071130</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A77" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="C71" s="12"/>
-      <c r="D71" s="12"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A72" s="11" t="s">
+      <c r="B77" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C77" s="16"/>
+      <c r="D77" s="16">
+        <v>20120131</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A78" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C72" s="12"/>
-      <c r="D72" s="12">
-        <v>20070831</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A73" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C73" s="12"/>
-      <c r="D73" s="12"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A74" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="C74" s="12"/>
-      <c r="D74" s="12">
-        <v>20110630</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A75" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12">
-        <v>20080530</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A76" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12">
-        <v>20071130</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A77" s="13" t="s">
-        <v>169</v>
-      </c>
-      <c r="B77" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="C77" s="14"/>
-      <c r="D77" s="14">
-        <v>20120131</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A78" s="13" t="s">
+      <c r="B78" s="13" t="s">
         <v>170</v>
-      </c>
-      <c r="B78" s="7" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.15">
@@ -2461,85 +2743,88 @@
       <c r="B79" s="1"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A81" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C81" s="11"/>
+      <c r="D81" s="11">
+        <v>20101029</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A82" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A83" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C83" s="11"/>
+      <c r="D83" s="11">
+        <v>20080630</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A84" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="C84" s="11"/>
+      <c r="D84" s="11">
+        <v>20091231</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A85" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="C85" s="11"/>
+      <c r="D85" s="11"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A86" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B80" s="4" t="s">
+      <c r="B86" s="4" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A81" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12">
-        <v>20101029</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A82" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A83" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C83" s="12"/>
-      <c r="D83" s="12">
-        <v>20080630</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A84" s="11" t="s">
+      <c r="C86" s="11"/>
+      <c r="D86" s="11">
+        <v>20090831</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A87" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B87" s="13" t="s">
         <v>187</v>
       </c>
-      <c r="C84" s="12"/>
-      <c r="D84" s="12">
-        <v>20091231</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A85" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="B85" s="1" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A86" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B86" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D86">
-        <v>20090831</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A87" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C87" s="14"/>
-      <c r="D87" s="14">
+      <c r="C87" s="16"/>
+      <c r="D87" s="16">
         <v>20110831</v>
       </c>
     </row>
@@ -2549,11 +2834,397 @@
     <row r="89" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A90" s="2"/>
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.15">
+      <c r="A90" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="B90" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C90" s="11" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A91" s="2"/>
+      <c r="A91" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C91" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D91" s="11">
+        <v>20110428</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A92" s="2"/>
+      <c r="B92" s="18"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A93" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="B93" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D93" s="11">
+        <v>20100528</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A94" s="10" t="s">
+        <v>195</v>
+      </c>
+      <c r="B94" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A95" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B95" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="D95" s="11">
+        <v>20070821</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A96" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="B96" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D96" s="11"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A97" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="B97" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C97" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A98" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="B98" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="C98" s="11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A99" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="B99" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="C99" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D99" s="11">
+        <v>20110104</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A100" s="10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B100" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="C100" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A101" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="B101" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C101" s="11" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A102" s="2"/>
+      <c r="B102" s="18"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A103" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="B103" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C103" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A104" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="B104" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="C104" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="D104">
+        <v>20070912</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A105" s="10"/>
+      <c r="B105" s="19"/>
+      <c r="C105" s="11"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A106" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B106" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C106" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A107" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B107" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C107" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D107" s="11">
+        <v>20091030</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A108" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B108" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C108" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="D108" s="11">
+        <v>20080630</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A109" s="10">
+        <v>600031</v>
+      </c>
+      <c r="B109" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="C109" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="D109" s="11"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A110" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B110" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C110" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D110" s="11">
+        <v>20091030</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A111" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B111" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C111" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="D111" s="11">
+        <v>20100331</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A112" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="B112" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="C112" s="11"/>
+      <c r="D112" s="11"/>
+    </row>
+    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A113" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="B113" s="20" t="s">
+        <v>235</v>
+      </c>
+      <c r="C113" s="11"/>
+      <c r="D113" s="11"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A114" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B114" s="19" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A115" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="B115" s="19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A116" s="2"/>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A117" s="2"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A118" s="2"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A119" s="2"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A120" s="2"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A121" s="2"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A122" s="2"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A123" s="2"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A124" s="2"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A125" s="2"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A126" s="2"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A127" s="2"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A128" s="2"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A129" s="2"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A130" s="2"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A131" s="2"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A132" s="2"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A133" s="2"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A134" s="2"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A135" s="2"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A136" s="2"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A137" s="2"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A138" s="2"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A139" s="2"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A140" s="2"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A141" s="2"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A142" s="2"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A143" s="2"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A144" s="2"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A145" s="2"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A146" s="2"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A147" s="2"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A148" s="2"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A149" s="2"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A150" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>